<commit_message>
add trap monster logic
</commit_message>
<xml_diff>
--- a/Assets/island/DBCfg/DataCfg.xlsx
+++ b/Assets/island/DBCfg/DataCfg.xlsx
@@ -691,7 +691,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="963">
   <si>
     <t>表名：</t>
   </si>
@@ -3040,31 +3040,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>800</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>400</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>200</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>800</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>400</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>200</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>100</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>快-&gt;慢-&gt;快</t>
-  </si>
-  <si>
-    <t>250</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>250</t>
@@ -4324,6 +4316,18 @@
   </si>
   <si>
     <t>8000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>battle.TrapMonsterAttack</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>250</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>200</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -10285,13 +10289,13 @@
         <v>402</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="8" customFormat="1" ht="15" customHeight="1">
@@ -10309,13 +10313,13 @@
         <v>403</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -10335,10 +10339,10 @@
         <v>5</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -10511,10 +10515,10 @@
   <dimension ref="A1:BM45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="AH15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="AG15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="AV30" sqref="AV30"/>
+      <selection pane="bottomRight" activeCell="AK31" sqref="AK31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10636,13 +10640,13 @@
         <v>42</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="L4" s="72" t="s">
         <v>516</v>
@@ -10741,19 +10745,19 @@
         <v>54</v>
       </c>
       <c r="AR4" s="116" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="AS4" s="116" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="AT4" s="116" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="AU4" s="30" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="AV4" s="102" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="AW4" s="30" t="s">
         <v>46</v>
@@ -10789,7 +10793,7 @@
         <v>57</v>
       </c>
       <c r="BH4" s="30" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="BI4" s="30" t="s">
         <v>58</v>
@@ -10818,7 +10822,7 @@
         <v>37</v>
       </c>
       <c r="E5" s="102" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>344</v>
@@ -10830,13 +10834,13 @@
         <v>69</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="L5" s="72" t="s">
         <v>518</v>
@@ -10848,7 +10852,7 @@
         <v>520</v>
       </c>
       <c r="O5" s="73" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="P5" s="73" t="s">
         <v>524</v>
@@ -10935,19 +10939,19 @@
         <v>80</v>
       </c>
       <c r="AR5" s="116" t="s">
+        <v>637</v>
+      </c>
+      <c r="AS5" s="116" t="s">
+        <v>638</v>
+      </c>
+      <c r="AT5" s="116" t="s">
         <v>639</v>
       </c>
-      <c r="AS5" s="116" t="s">
-        <v>640</v>
-      </c>
-      <c r="AT5" s="116" t="s">
-        <v>641</v>
-      </c>
       <c r="AU5" s="49" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="AV5" s="169" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="AW5" s="28" t="s">
         <v>73</v>
@@ -10959,7 +10963,7 @@
         <v>75</v>
       </c>
       <c r="AZ5" s="28" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="BA5" s="109" t="s">
         <v>70</v>
@@ -10968,22 +10972,22 @@
         <v>81</v>
       </c>
       <c r="BC5" s="28" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="BD5" s="28" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="BE5" s="28" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="BF5" s="28" t="s">
         <v>76</v>
       </c>
       <c r="BG5" s="28" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="BH5" s="28" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="BI5" s="28" t="s">
         <v>83</v>
@@ -11141,7 +11145,7 @@
         <v>5</v>
       </c>
       <c r="AV6" s="102" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="AW6" s="30" t="s">
         <v>89</v>
@@ -11207,13 +11211,13 @@
         <v>91</v>
       </c>
       <c r="D7" s="104" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="E7" s="103" t="s">
         <v>347</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="G7" s="35" t="s">
         <v>94</v>
@@ -11223,10 +11227,10 @@
       </c>
       <c r="I7" s="35"/>
       <c r="J7" s="35" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="K7" s="35" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="L7" s="79">
         <v>0</v>
@@ -11236,7 +11240,7 @@
         <v>17280</v>
       </c>
       <c r="N7" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O7" s="76">
         <v>0</v>
@@ -11245,7 +11249,7 @@
         <v>552</v>
       </c>
       <c r="Q7" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R7" s="90">
         <v>0</v>
@@ -11254,7 +11258,7 @@
         <v>30000000</v>
       </c>
       <c r="T7" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U7" s="88">
         <v>0</v>
@@ -11263,7 +11267,7 @@
         <v>30000000</v>
       </c>
       <c r="W7" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X7" s="81">
         <v>1500</v>
@@ -11308,7 +11312,7 @@
       <c r="BB7" s="35"/>
       <c r="BC7" s="35"/>
       <c r="BD7" s="31" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="BE7" s="31"/>
       <c r="BF7" s="35"/>
@@ -11350,10 +11354,10 @@
       </c>
       <c r="I8" s="35"/>
       <c r="J8" s="35" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="K8" s="35" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="L8" s="79" t="s">
         <v>92</v>
@@ -11362,7 +11366,7 @@
         <v>5760</v>
       </c>
       <c r="N8" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O8" s="76" t="s">
         <v>117</v>
@@ -11371,7 +11375,7 @@
         <v>540</v>
       </c>
       <c r="Q8" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R8" s="90" t="s">
         <v>117</v>
@@ -11380,7 +11384,7 @@
         <v>540</v>
       </c>
       <c r="T8" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U8" s="88" t="s">
         <v>117</v>
@@ -11389,7 +11393,7 @@
         <v>540</v>
       </c>
       <c r="W8" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X8" s="82">
         <v>250</v>
@@ -11425,10 +11429,10 @@
         <v>548</v>
       </c>
       <c r="AM8" s="114" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="AN8" s="114" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="AO8" s="115" t="s">
         <v>548</v>
@@ -11452,7 +11456,7 @@
       <c r="BB8" s="35"/>
       <c r="BC8" s="35"/>
       <c r="BD8" s="31" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="BE8" s="31"/>
       <c r="BF8" s="35"/>
@@ -11494,10 +11498,10 @@
       </c>
       <c r="I9" s="35"/>
       <c r="J9" s="35" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="K9" s="35" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="L9" s="79">
         <v>1</v>
@@ -11506,7 +11510,7 @@
         <v>5760</v>
       </c>
       <c r="N9" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O9" s="76" t="s">
         <v>104</v>
@@ -11515,7 +11519,7 @@
         <v>540</v>
       </c>
       <c r="Q9" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R9" s="90" t="s">
         <v>104</v>
@@ -11524,7 +11528,7 @@
         <v>540</v>
       </c>
       <c r="T9" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U9" s="88" t="s">
         <v>104</v>
@@ -11533,7 +11537,7 @@
         <v>540</v>
       </c>
       <c r="W9" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X9" s="81" t="s">
         <v>106</v>
@@ -11578,7 +11582,7 @@
       <c r="BB9" s="35"/>
       <c r="BC9" s="35"/>
       <c r="BD9" s="36" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="BE9" s="36"/>
       <c r="BF9" s="35"/>
@@ -11620,10 +11624,10 @@
       </c>
       <c r="I10" s="35"/>
       <c r="J10" s="35" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="K10" s="35" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="L10" s="79">
         <v>1</v>
@@ -11632,7 +11636,7 @@
         <v>5760</v>
       </c>
       <c r="N10" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O10" s="76" t="s">
         <v>108</v>
@@ -11641,7 +11645,7 @@
         <v>540</v>
       </c>
       <c r="Q10" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R10" s="90" t="s">
         <v>108</v>
@@ -11650,7 +11654,7 @@
         <v>540</v>
       </c>
       <c r="T10" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U10" s="88" t="s">
         <v>108</v>
@@ -11659,7 +11663,7 @@
         <v>540</v>
       </c>
       <c r="W10" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X10" s="82">
         <v>500</v>
@@ -11716,7 +11720,7 @@
       <c r="BB10" s="35"/>
       <c r="BC10" s="35"/>
       <c r="BD10" s="36" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="BE10" s="36"/>
       <c r="BF10" s="35"/>
@@ -11758,10 +11762,10 @@
       </c>
       <c r="I11" s="35"/>
       <c r="J11" s="35" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="K11" s="35" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="L11" s="79">
         <v>1</v>
@@ -11770,7 +11774,7 @@
         <v>5760</v>
       </c>
       <c r="N11" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O11" s="76">
         <v>0</v>
@@ -11779,7 +11783,7 @@
         <v>540</v>
       </c>
       <c r="Q11" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R11" s="90">
         <v>0</v>
@@ -11788,7 +11792,7 @@
         <v>540</v>
       </c>
       <c r="T11" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U11" s="88">
         <v>0</v>
@@ -11797,7 +11801,7 @@
         <v>540</v>
       </c>
       <c r="W11" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X11" s="82">
         <v>580</v>
@@ -11848,7 +11852,7 @@
       <c r="BB11" s="36"/>
       <c r="BC11" s="36"/>
       <c r="BD11" s="31" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="BE11" s="36"/>
       <c r="BF11" s="36"/>
@@ -11890,10 +11894,10 @@
       </c>
       <c r="I12" s="35"/>
       <c r="J12" s="35" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="K12" s="35" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="L12" s="79">
         <v>1</v>
@@ -11902,7 +11906,7 @@
         <v>10080</v>
       </c>
       <c r="N12" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O12" s="76"/>
       <c r="P12" s="76"/>
@@ -11914,7 +11918,7 @@
         <v>539</v>
       </c>
       <c r="T12" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U12" s="88" t="s">
         <v>133</v>
@@ -11923,7 +11927,7 @@
         <v>539</v>
       </c>
       <c r="W12" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X12" s="81">
         <v>400</v>
@@ -11974,10 +11978,10 @@
       <c r="BB12" s="35"/>
       <c r="BC12" s="35"/>
       <c r="BD12" s="36" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="BE12" s="37" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="BF12" s="35"/>
       <c r="BG12" s="35"/>
@@ -12018,10 +12022,10 @@
       </c>
       <c r="I13" s="35"/>
       <c r="J13" s="35" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="K13" s="35" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="L13" s="79">
         <v>1</v>
@@ -12030,7 +12034,7 @@
         <v>10080</v>
       </c>
       <c r="N13" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O13" s="76"/>
       <c r="P13" s="76"/>
@@ -12042,7 +12046,7 @@
         <v>539</v>
       </c>
       <c r="T13" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U13" s="88" t="s">
         <v>141</v>
@@ -12051,7 +12055,7 @@
         <v>539</v>
       </c>
       <c r="W13" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X13" s="81" t="s">
         <v>114</v>
@@ -12100,7 +12104,7 @@
       <c r="BB13" s="35"/>
       <c r="BC13" s="35"/>
       <c r="BD13" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="BE13" s="33"/>
       <c r="BF13" s="35"/>
@@ -12142,10 +12146,10 @@
       </c>
       <c r="I14" s="35"/>
       <c r="J14" s="35" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="K14" s="35" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="L14" s="79">
         <v>1</v>
@@ -12154,7 +12158,7 @@
         <v>10080</v>
       </c>
       <c r="N14" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O14" s="76" t="s">
         <v>133</v>
@@ -12163,7 +12167,7 @@
         <v>539</v>
       </c>
       <c r="Q14" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R14" s="90"/>
       <c r="S14" s="90"/>
@@ -12175,7 +12179,7 @@
         <v>539</v>
       </c>
       <c r="W14" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X14" s="81">
         <v>400</v>
@@ -12226,10 +12230,10 @@
       <c r="BB14" s="35"/>
       <c r="BC14" s="35"/>
       <c r="BD14" s="36" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="BE14" s="37" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="BF14" s="35"/>
       <c r="BG14" s="35"/>
@@ -12270,10 +12274,10 @@
       </c>
       <c r="I15" s="35"/>
       <c r="J15" s="35" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="K15" s="35" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="L15" s="79">
         <v>1</v>
@@ -12282,7 +12286,7 @@
         <v>10080</v>
       </c>
       <c r="N15" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O15" s="76" t="s">
         <v>141</v>
@@ -12291,7 +12295,7 @@
         <v>539</v>
       </c>
       <c r="Q15" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R15" s="90"/>
       <c r="S15" s="90"/>
@@ -12303,7 +12307,7 @@
         <v>539</v>
       </c>
       <c r="W15" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X15" s="81" t="s">
         <v>114</v>
@@ -12318,7 +12322,7 @@
         <v>614</v>
       </c>
       <c r="AB15" s="92" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="AC15" s="93" t="s">
         <v>548</v>
@@ -12352,7 +12356,7 @@
       <c r="BB15" s="35"/>
       <c r="BC15" s="35"/>
       <c r="BD15" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="BE15" s="33"/>
       <c r="BF15" s="35"/>
@@ -12394,10 +12398,10 @@
       </c>
       <c r="I16" s="35"/>
       <c r="J16" s="35" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="K16" s="35" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="L16" s="79">
         <v>1</v>
@@ -12406,7 +12410,7 @@
         <v>10080</v>
       </c>
       <c r="N16" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O16" s="76">
         <v>150</v>
@@ -12415,7 +12419,7 @@
         <v>539</v>
       </c>
       <c r="Q16" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R16" s="90">
         <v>150</v>
@@ -12424,7 +12428,7 @@
         <v>539</v>
       </c>
       <c r="T16" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U16" s="88"/>
       <c r="V16" s="88"/>
@@ -12478,10 +12482,10 @@
       <c r="BB16" s="35"/>
       <c r="BC16" s="35"/>
       <c r="BD16" s="31" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="BE16" s="33" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="BF16" s="35"/>
       <c r="BG16" s="35"/>
@@ -12522,10 +12526,10 @@
       </c>
       <c r="I17" s="35"/>
       <c r="J17" s="35" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="K17" s="35" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="L17" s="79">
         <v>1</v>
@@ -12534,7 +12538,7 @@
         <v>10080</v>
       </c>
       <c r="N17" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O17" s="76" t="s">
         <v>141</v>
@@ -12543,7 +12547,7 @@
         <v>539</v>
       </c>
       <c r="Q17" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R17" s="90" t="s">
         <v>141</v>
@@ -12552,7 +12556,7 @@
         <v>539</v>
       </c>
       <c r="T17" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U17" s="88"/>
       <c r="V17" s="88"/>
@@ -12604,7 +12608,7 @@
       <c r="BB17" s="35"/>
       <c r="BC17" s="35"/>
       <c r="BD17" s="31" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="BE17" s="33"/>
       <c r="BF17" s="35"/>
@@ -12646,10 +12650,10 @@
       </c>
       <c r="I18" s="35"/>
       <c r="J18" s="35" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="K18" s="35" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="L18" s="79">
         <f>60/60</f>
@@ -12659,7 +12663,7 @@
         <v>10080</v>
       </c>
       <c r="N18" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O18" s="76">
         <v>250</v>
@@ -12668,7 +12672,7 @@
         <v>554</v>
       </c>
       <c r="Q18" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R18" s="90">
         <v>250</v>
@@ -12677,7 +12681,7 @@
         <v>539</v>
       </c>
       <c r="T18" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U18" s="88">
         <v>250</v>
@@ -12686,7 +12690,7 @@
         <v>539</v>
       </c>
       <c r="W18" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X18" s="81">
         <v>400</v>
@@ -12726,7 +12730,7 @@
         <v>7</v>
       </c>
       <c r="AS18" s="117" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="AT18" s="118" t="s">
         <v>548</v>
@@ -12747,12 +12751,12 @@
       <c r="BB18" s="34"/>
       <c r="BC18" s="34"/>
       <c r="BD18" s="34" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="BE18" s="34"/>
       <c r="BF18" s="34"/>
       <c r="BG18" s="34" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="BH18" s="34"/>
       <c r="BI18" s="34" t="s">
@@ -12795,10 +12799,10 @@
       </c>
       <c r="I19" s="35"/>
       <c r="J19" s="35" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="K19" s="35" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="L19" s="79">
         <f t="shared" ref="L19:L31" si="1">60/60</f>
@@ -12808,7 +12812,7 @@
         <v>10080</v>
       </c>
       <c r="N19" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O19" s="76">
         <v>1000</v>
@@ -12817,7 +12821,7 @@
         <v>554</v>
       </c>
       <c r="Q19" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R19" s="90">
         <v>1000</v>
@@ -12826,7 +12830,7 @@
         <v>539</v>
       </c>
       <c r="T19" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U19" s="88">
         <v>1000</v>
@@ -12835,7 +12839,7 @@
         <v>539</v>
       </c>
       <c r="W19" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X19" s="81">
         <v>400</v>
@@ -12875,7 +12879,7 @@
         <v>11</v>
       </c>
       <c r="AS19" s="117" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="AT19" s="118" t="s">
         <v>548</v>
@@ -12896,12 +12900,12 @@
       <c r="BB19" s="32"/>
       <c r="BC19" s="32"/>
       <c r="BD19" s="36" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="BE19" s="36"/>
       <c r="BF19" s="32"/>
       <c r="BG19" s="36" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="BH19" s="36"/>
       <c r="BI19" s="35" t="s">
@@ -12944,10 +12948,10 @@
       </c>
       <c r="I20" s="35"/>
       <c r="J20" s="35" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="K20" s="35" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="L20" s="79">
         <f t="shared" si="1"/>
@@ -12957,7 +12961,7 @@
         <v>10080</v>
       </c>
       <c r="N20" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O20" s="76" t="s">
         <v>162</v>
@@ -12966,7 +12970,7 @@
         <v>554</v>
       </c>
       <c r="Q20" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R20" s="90" t="s">
         <v>162</v>
@@ -12975,7 +12979,7 @@
         <v>539</v>
       </c>
       <c r="T20" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U20" s="88" t="s">
         <v>162</v>
@@ -12984,7 +12988,7 @@
         <v>539</v>
       </c>
       <c r="W20" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X20" s="81">
         <v>400</v>
@@ -13017,22 +13021,22 @@
         <v>548</v>
       </c>
       <c r="AP20" s="35" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="AQ20" s="34" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="AR20" s="117">
         <v>20</v>
       </c>
       <c r="AS20" s="117" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="AT20" s="118" t="s">
         <v>576</v>
       </c>
       <c r="AU20" s="36" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="AV20" s="36"/>
       <c r="AW20" s="34"/>
@@ -13049,12 +13053,12 @@
       <c r="BB20" s="34"/>
       <c r="BC20" s="34"/>
       <c r="BD20" s="34" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="BE20" s="34"/>
       <c r="BF20" s="34"/>
       <c r="BG20" s="34" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="BH20" s="34"/>
       <c r="BI20" s="34" t="s">
@@ -13097,10 +13101,10 @@
       </c>
       <c r="I21" s="35"/>
       <c r="J21" s="35" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="K21" s="35" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="L21" s="79">
         <f t="shared" si="1"/>
@@ -13110,7 +13114,7 @@
         <v>10080</v>
       </c>
       <c r="N21" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O21" s="76">
         <v>22500</v>
@@ -13119,7 +13123,7 @@
         <v>554</v>
       </c>
       <c r="Q21" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R21" s="90">
         <v>22500</v>
@@ -13128,7 +13132,7 @@
         <v>539</v>
       </c>
       <c r="T21" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U21" s="88">
         <v>22500</v>
@@ -13137,7 +13141,7 @@
         <v>539</v>
       </c>
       <c r="W21" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X21" s="81" t="s">
         <v>577</v>
@@ -13161,10 +13165,10 @@
       <c r="AK21" s="106"/>
       <c r="AL21" s="107"/>
       <c r="AM21" s="114" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="AN21" s="114" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="AO21" s="115" t="s">
         <v>548</v>
@@ -13177,7 +13181,7 @@
         <v>80</v>
       </c>
       <c r="AS21" s="117" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="AT21" s="118" t="s">
         <v>576</v>
@@ -13190,7 +13194,7 @@
         <v>94</v>
       </c>
       <c r="AZ21" s="32" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="BA21" s="111" t="s">
         <v>619</v>
@@ -13198,12 +13202,12 @@
       <c r="BB21" s="32"/>
       <c r="BC21" s="32"/>
       <c r="BD21" s="36" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="BE21" s="36"/>
       <c r="BF21" s="32"/>
       <c r="BG21" s="36" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="BH21" s="36"/>
       <c r="BI21" s="32" t="s">
@@ -13227,7 +13231,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D22" s="104" t="s">
         <v>390</v>
@@ -13246,10 +13250,10 @@
       </c>
       <c r="I22" s="35"/>
       <c r="J22" s="35" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="K22" s="35" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="L22" s="79">
         <f t="shared" si="1"/>
@@ -13259,7 +13263,7 @@
         <v>10080</v>
       </c>
       <c r="N22" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O22" s="77" t="s">
         <v>168</v>
@@ -13268,7 +13272,7 @@
         <v>554</v>
       </c>
       <c r="Q22" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R22" s="90" t="s">
         <v>168</v>
@@ -13277,7 +13281,7 @@
         <v>553</v>
       </c>
       <c r="T22" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U22" s="88" t="s">
         <v>168</v>
@@ -13286,7 +13290,7 @@
         <v>553</v>
       </c>
       <c r="W22" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X22" s="82" t="s">
         <v>578</v>
@@ -13310,31 +13314,31 @@
       <c r="AK22" s="106"/>
       <c r="AL22" s="107"/>
       <c r="AM22" s="114" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="AN22" s="114" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="AO22" s="115" t="s">
         <v>548</v>
       </c>
       <c r="AP22" s="35" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="AQ22" s="34" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="AR22" s="119" t="s">
         <v>169</v>
       </c>
       <c r="AS22" s="119" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="AT22" s="118" t="s">
         <v>548</v>
       </c>
       <c r="AU22" s="36" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="AV22" s="36"/>
       <c r="AW22" s="34"/>
@@ -13343,7 +13347,7 @@
         <v>94</v>
       </c>
       <c r="AZ22" s="34" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="BA22" s="111" t="s">
         <v>619</v>
@@ -13351,12 +13355,12 @@
       <c r="BB22" s="34"/>
       <c r="BC22" s="34"/>
       <c r="BD22" s="34" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="BE22" s="34"/>
       <c r="BF22" s="34"/>
       <c r="BG22" s="36" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="BH22" s="36"/>
       <c r="BI22" s="34" t="s">
@@ -13380,7 +13384,7 @@
         <v>17</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="D23" s="104" t="s">
         <v>179</v>
@@ -13399,10 +13403,10 @@
       </c>
       <c r="I23" s="35"/>
       <c r="J23" s="35" t="s">
+        <v>724</v>
+      </c>
+      <c r="K23" s="35" t="s">
         <v>726</v>
-      </c>
-      <c r="K23" s="35" t="s">
-        <v>728</v>
       </c>
       <c r="L23" s="79">
         <f t="shared" si="1"/>
@@ -13412,7 +13416,7 @@
         <v>10080</v>
       </c>
       <c r="N23" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O23" s="76" t="s">
         <v>549</v>
@@ -13421,7 +13425,7 @@
         <v>555</v>
       </c>
       <c r="Q23" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R23" s="90" t="s">
         <v>549</v>
@@ -13430,7 +13434,7 @@
         <v>550</v>
       </c>
       <c r="T23" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U23" s="88" t="s">
         <v>549</v>
@@ -13439,7 +13443,7 @@
         <v>550</v>
       </c>
       <c r="W23" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X23" s="81" t="s">
         <v>557</v>
@@ -13479,7 +13483,7 @@
         <v>20</v>
       </c>
       <c r="AS23" s="117" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="AT23" s="118" t="s">
         <v>547</v>
@@ -13500,12 +13504,12 @@
       <c r="BB23" s="32"/>
       <c r="BC23" s="32"/>
       <c r="BD23" s="36" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="BE23" s="36"/>
       <c r="BF23" s="32"/>
       <c r="BG23" s="32" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="BH23" s="32"/>
       <c r="BI23" s="32" t="s">
@@ -13548,10 +13552,10 @@
       </c>
       <c r="I24" s="35"/>
       <c r="J24" s="35" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="K24" s="35" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="L24" s="79">
         <f t="shared" si="1"/>
@@ -13562,7 +13566,7 @@
         <v>17280</v>
       </c>
       <c r="N24" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O24" s="76">
         <v>2500000</v>
@@ -13571,7 +13575,7 @@
         <v>550</v>
       </c>
       <c r="Q24" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R24" s="90">
         <v>2500000</v>
@@ -13580,7 +13584,7 @@
         <v>551</v>
       </c>
       <c r="T24" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U24" s="88">
         <v>2500000</v>
@@ -13589,7 +13593,7 @@
         <v>551</v>
       </c>
       <c r="W24" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X24" s="81">
         <v>1500</v>
@@ -13625,13 +13629,13 @@
         <v>183</v>
       </c>
       <c r="AQ24" s="36" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="AR24" s="117" t="s">
         <v>177</v>
       </c>
       <c r="AS24" s="117" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="AT24" s="118" t="s">
         <v>569</v>
@@ -13652,12 +13656,12 @@
       <c r="BB24" s="36"/>
       <c r="BC24" s="36"/>
       <c r="BD24" s="31" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="BE24" s="36"/>
       <c r="BF24" s="36"/>
       <c r="BG24" s="36" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="BH24" s="36"/>
       <c r="BI24" s="32" t="s">
@@ -13702,10 +13706,10 @@
         <v>94</v>
       </c>
       <c r="J25" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K25" s="35" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="L25" s="79">
         <f t="shared" si="1"/>
@@ -13715,7 +13719,7 @@
         <v>10080</v>
       </c>
       <c r="N25" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O25" s="76" t="s">
         <v>188</v>
@@ -13724,7 +13728,7 @@
         <v>539</v>
       </c>
       <c r="Q25" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R25" s="90" t="s">
         <v>188</v>
@@ -13733,7 +13737,7 @@
         <v>539</v>
       </c>
       <c r="T25" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U25" s="88" t="s">
         <v>188</v>
@@ -13742,7 +13746,7 @@
         <v>539</v>
       </c>
       <c r="W25" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X25" s="83"/>
       <c r="Y25" s="83"/>
@@ -13757,19 +13761,19 @@
       <c r="AH25" s="98"/>
       <c r="AI25" s="99"/>
       <c r="AJ25" s="38" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="AK25" s="38" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="AL25" s="107" t="s">
         <v>548</v>
       </c>
       <c r="AM25" s="114" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AN25" s="114" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="AO25" s="115" t="s">
         <v>548</v>
@@ -13782,7 +13786,7 @@
         <v>190</v>
       </c>
       <c r="AS25" s="120" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="AT25" s="118" t="s">
         <v>547</v>
@@ -13803,13 +13807,13 @@
       <c r="BB25" s="38"/>
       <c r="BC25" s="38"/>
       <c r="BD25" s="31" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="BE25" s="36"/>
       <c r="BF25" s="36"/>
       <c r="BG25" s="36"/>
       <c r="BH25" s="36" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="BI25" s="38" t="s">
         <v>119</v>
@@ -13832,7 +13836,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="35" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D26" s="104" t="s">
         <v>392</v>
@@ -13853,10 +13857,10 @@
         <v>94</v>
       </c>
       <c r="J26" s="35" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L26" s="79">
         <f t="shared" si="1"/>
@@ -13866,7 +13870,7 @@
         <v>10080</v>
       </c>
       <c r="N26" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O26" s="76" t="s">
         <v>114</v>
@@ -13875,7 +13879,7 @@
         <v>539</v>
       </c>
       <c r="Q26" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R26" s="90" t="s">
         <v>114</v>
@@ -13884,7 +13888,7 @@
         <v>539</v>
       </c>
       <c r="T26" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U26" s="88" t="s">
         <v>114</v>
@@ -13893,7 +13897,7 @@
         <v>539</v>
       </c>
       <c r="W26" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X26" s="83"/>
       <c r="Y26" s="83"/>
@@ -13908,32 +13912,32 @@
       <c r="AH26" s="98"/>
       <c r="AI26" s="99"/>
       <c r="AJ26" s="36" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="AK26" s="36" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="AL26" s="107" t="s">
         <v>548</v>
       </c>
       <c r="AM26" s="114" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AN26" s="114" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AO26" s="115" t="s">
         <v>548</v>
       </c>
       <c r="AP26" s="35"/>
       <c r="AQ26" s="36" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="AR26" s="120" t="s">
         <v>124</v>
       </c>
       <c r="AS26" s="120" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="AT26" s="118" t="s">
         <v>576</v>
@@ -13954,13 +13958,13 @@
       <c r="BB26" s="36"/>
       <c r="BC26" s="36"/>
       <c r="BD26" s="31" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="BE26" s="36"/>
       <c r="BF26" s="36"/>
       <c r="BG26" s="36"/>
       <c r="BH26" s="36" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="BI26" s="32" t="s">
         <v>94</v>
@@ -14004,10 +14008,10 @@
         <v>94</v>
       </c>
       <c r="J27" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K27" s="35" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="L27" s="79">
         <f t="shared" si="1"/>
@@ -14017,7 +14021,7 @@
         <v>10080</v>
       </c>
       <c r="N27" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O27" s="76" t="s">
         <v>188</v>
@@ -14026,7 +14030,7 @@
         <v>539</v>
       </c>
       <c r="Q27" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R27" s="90" t="s">
         <v>188</v>
@@ -14035,7 +14039,7 @@
         <v>539</v>
       </c>
       <c r="T27" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U27" s="88" t="s">
         <v>188</v>
@@ -14044,7 +14048,7 @@
         <v>539</v>
       </c>
       <c r="W27" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X27" s="83"/>
       <c r="Y27" s="83"/>
@@ -14059,7 +14063,7 @@
       <c r="AH27" s="98"/>
       <c r="AI27" s="99"/>
       <c r="AJ27" s="36" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="AK27" s="36" t="s">
         <v>117</v>
@@ -14068,10 +14072,10 @@
         <v>548</v>
       </c>
       <c r="AM27" s="114" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AN27" s="114" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AO27" s="115" t="s">
         <v>548</v>
@@ -14084,7 +14088,7 @@
         <v>190</v>
       </c>
       <c r="AS27" s="120" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="AT27" s="118" t="s">
         <v>548</v>
@@ -14105,13 +14109,13 @@
       <c r="BB27" s="36"/>
       <c r="BC27" s="36"/>
       <c r="BD27" s="31" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="BE27" s="36"/>
       <c r="BF27" s="36"/>
       <c r="BG27" s="36"/>
       <c r="BH27" s="36" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="BI27" s="36" t="s">
         <v>119</v>
@@ -14134,7 +14138,7 @@
         <v>22</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D28" s="104" t="s">
         <v>393</v>
@@ -14155,10 +14159,10 @@
         <v>94</v>
       </c>
       <c r="J28" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K28" s="35" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="L28" s="79">
         <f t="shared" si="1"/>
@@ -14168,7 +14172,7 @@
         <v>10080</v>
       </c>
       <c r="N28" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O28" s="76" t="s">
         <v>145</v>
@@ -14177,7 +14181,7 @@
         <v>539</v>
       </c>
       <c r="Q28" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R28" s="90" t="s">
         <v>145</v>
@@ -14186,7 +14190,7 @@
         <v>539</v>
       </c>
       <c r="T28" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U28" s="88" t="s">
         <v>145</v>
@@ -14195,7 +14199,7 @@
         <v>539</v>
       </c>
       <c r="W28" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X28" s="83"/>
       <c r="Y28" s="83"/>
@@ -14204,7 +14208,7 @@
         <v>122</v>
       </c>
       <c r="AB28" s="92" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="AC28" s="93" t="s">
         <v>548</v>
@@ -14225,7 +14229,7 @@
         <v>548</v>
       </c>
       <c r="AM28" s="114" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="AN28" s="114" t="s">
         <v>189</v>
@@ -14238,17 +14242,17 @@
         <v>189</v>
       </c>
       <c r="AR28" s="120" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="AS28" s="120" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="AT28" s="118" t="s">
         <v>548</v>
       </c>
       <c r="AU28" s="36"/>
       <c r="AV28" s="36" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="AW28" s="35" t="s">
         <v>94</v>
@@ -14262,7 +14266,7 @@
       <c r="BB28" s="36"/>
       <c r="BC28" s="36"/>
       <c r="BD28" s="31" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="BE28" s="36"/>
       <c r="BF28" s="36"/>
@@ -14310,10 +14314,10 @@
         <v>94</v>
       </c>
       <c r="J29" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K29" s="35" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L29" s="79">
         <f t="shared" si="1"/>
@@ -14323,7 +14327,7 @@
         <v>10080</v>
       </c>
       <c r="N29" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O29" s="76" t="s">
         <v>203</v>
@@ -14332,7 +14336,7 @@
         <v>539</v>
       </c>
       <c r="Q29" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R29" s="90" t="s">
         <v>203</v>
@@ -14341,7 +14345,7 @@
         <v>539</v>
       </c>
       <c r="T29" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U29" s="88" t="s">
         <v>203</v>
@@ -14350,7 +14354,7 @@
         <v>539</v>
       </c>
       <c r="W29" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X29" s="83"/>
       <c r="Y29" s="83"/>
@@ -14359,7 +14363,7 @@
         <v>158</v>
       </c>
       <c r="AB29" s="92" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="AC29" s="93" t="s">
         <v>548</v>
@@ -14371,39 +14375,39 @@
       <c r="AH29" s="98"/>
       <c r="AI29" s="99"/>
       <c r="AJ29" s="36" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="AK29" s="36" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AL29" s="107" t="s">
         <v>548</v>
       </c>
       <c r="AM29" s="114" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AN29" s="114" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="AO29" s="115" t="s">
         <v>548</v>
       </c>
       <c r="AP29" s="35"/>
       <c r="AQ29" s="38" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="AR29" s="120" t="s">
         <v>92</v>
       </c>
       <c r="AS29" s="120" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="AT29" s="118" t="s">
         <v>548</v>
       </c>
       <c r="AU29" s="36"/>
       <c r="AV29" s="36" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="AW29" s="35" t="s">
         <v>94</v>
@@ -14417,13 +14421,13 @@
       <c r="BB29" s="36"/>
       <c r="BC29" s="36"/>
       <c r="BD29" s="31" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="BE29" s="36"/>
       <c r="BF29" s="36"/>
       <c r="BG29" s="36"/>
       <c r="BH29" s="36" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="BI29" s="32" t="s">
         <v>94</v>
@@ -14476,7 +14480,7 @@
         <v>10080</v>
       </c>
       <c r="N30" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O30" s="76" t="s">
         <v>128</v>
@@ -14485,7 +14489,7 @@
         <v>539</v>
       </c>
       <c r="Q30" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R30" s="90" t="s">
         <v>128</v>
@@ -14494,7 +14498,7 @@
         <v>539</v>
       </c>
       <c r="T30" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U30" s="88" t="s">
         <v>128</v>
@@ -14503,7 +14507,7 @@
         <v>539</v>
       </c>
       <c r="W30" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X30" s="83"/>
       <c r="Y30" s="83"/>
@@ -14521,7 +14525,7 @@
         <v>124</v>
       </c>
       <c r="AK30" s="36" t="s">
-        <v>636</v>
+        <v>962</v>
       </c>
       <c r="AL30" s="107" t="s">
         <v>548</v>
@@ -14530,20 +14534,20 @@
         <v>124</v>
       </c>
       <c r="AN30" s="114" t="s">
-        <v>630</v>
+        <v>961</v>
       </c>
       <c r="AO30" s="115" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AP30" s="35"/>
       <c r="AQ30" s="38" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="AR30" s="120" t="s">
         <v>96</v>
       </c>
       <c r="AS30" s="120" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="AT30" s="118" t="s">
         <v>548</v>
@@ -14562,12 +14566,14 @@
       <c r="BB30" s="36"/>
       <c r="BC30" s="36"/>
       <c r="BD30" s="31" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="BE30" s="36"/>
       <c r="BF30" s="36"/>
       <c r="BG30" s="36"/>
-      <c r="BH30" s="36"/>
+      <c r="BH30" s="36" t="s">
+        <v>960</v>
+      </c>
       <c r="BI30" s="32" t="s">
         <v>119</v>
       </c>
@@ -14610,10 +14616,10 @@
         <v>94</v>
       </c>
       <c r="J31" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K31" s="35" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L31" s="79">
         <f t="shared" si="1"/>
@@ -14623,7 +14629,7 @@
         <v>10080</v>
       </c>
       <c r="N31" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O31" s="76" t="s">
         <v>130</v>
@@ -14632,7 +14638,7 @@
         <v>539</v>
       </c>
       <c r="Q31" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R31" s="90" t="s">
         <v>130</v>
@@ -14641,7 +14647,7 @@
         <v>539</v>
       </c>
       <c r="T31" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U31" s="88" t="s">
         <v>130</v>
@@ -14650,7 +14656,7 @@
         <v>539</v>
       </c>
       <c r="W31" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X31" s="83"/>
       <c r="Y31" s="83"/>
@@ -14659,7 +14665,7 @@
         <v>158</v>
       </c>
       <c r="AB31" s="92" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="AC31" s="93" t="s">
         <v>548</v>
@@ -14671,10 +14677,10 @@
       <c r="AH31" s="98"/>
       <c r="AI31" s="99"/>
       <c r="AJ31" s="36" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="AK31" s="36" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="AL31" s="107" t="s">
         <v>548</v>
@@ -14703,7 +14709,7 @@
       </c>
       <c r="AU31" s="36"/>
       <c r="AV31" s="36" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="AW31" s="35" t="s">
         <v>94</v>
@@ -14717,7 +14723,7 @@
       <c r="BB31" s="36"/>
       <c r="BC31" s="36"/>
       <c r="BD31" s="31" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="BE31" s="36"/>
       <c r="BF31" s="36"/>
@@ -14753,7 +14759,7 @@
         <v>92</v>
       </c>
       <c r="F32" s="35" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G32" s="35" t="s">
         <v>119</v>
@@ -14774,7 +14780,7 @@
         <v>100000</v>
       </c>
       <c r="Q32" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R32" s="90"/>
       <c r="S32" s="90"/>
@@ -14786,7 +14792,7 @@
         <v>100000</v>
       </c>
       <c r="W32" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X32" s="82"/>
       <c r="Y32" s="82"/>
@@ -14821,7 +14827,7 @@
       <c r="BB32" s="36"/>
       <c r="BC32" s="36"/>
       <c r="BD32" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE32" s="36"/>
       <c r="BF32" s="36"/>
@@ -14853,7 +14859,7 @@
         <v>92</v>
       </c>
       <c r="F33" s="35" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G33" s="35" t="s">
         <v>119</v>
@@ -14874,7 +14880,7 @@
         <v>100000</v>
       </c>
       <c r="Q33" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R33" s="90"/>
       <c r="S33" s="90"/>
@@ -14886,7 +14892,7 @@
         <v>100000</v>
       </c>
       <c r="W33" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X33" s="82"/>
       <c r="Y33" s="82"/>
@@ -14921,7 +14927,7 @@
       <c r="BB33" s="36"/>
       <c r="BC33" s="36"/>
       <c r="BD33" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE33" s="36"/>
       <c r="BF33" s="36"/>
@@ -14953,7 +14959,7 @@
         <v>92</v>
       </c>
       <c r="F34" s="35" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G34" s="35" t="s">
         <v>119</v>
@@ -14974,7 +14980,7 @@
         <v>100000</v>
       </c>
       <c r="Q34" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R34" s="90"/>
       <c r="S34" s="90"/>
@@ -14986,7 +14992,7 @@
         <v>100000</v>
       </c>
       <c r="W34" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X34" s="82"/>
       <c r="Y34" s="82"/>
@@ -15021,7 +15027,7 @@
       <c r="BB34" s="36"/>
       <c r="BC34" s="36"/>
       <c r="BD34" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE34" s="36"/>
       <c r="BF34" s="36"/>
@@ -15053,7 +15059,7 @@
         <v>92</v>
       </c>
       <c r="F35" s="35" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G35" s="35" t="s">
         <v>119</v>
@@ -15074,7 +15080,7 @@
         <v>100000</v>
       </c>
       <c r="Q35" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R35" s="90"/>
       <c r="S35" s="90"/>
@@ -15086,7 +15092,7 @@
         <v>100000</v>
       </c>
       <c r="W35" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X35" s="82"/>
       <c r="Y35" s="82"/>
@@ -15121,7 +15127,7 @@
       <c r="BB35" s="36"/>
       <c r="BC35" s="36"/>
       <c r="BD35" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE35" s="36"/>
       <c r="BF35" s="36"/>
@@ -15153,7 +15159,7 @@
         <v>92</v>
       </c>
       <c r="F36" s="35" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G36" s="35" t="s">
         <v>119</v>
@@ -15174,7 +15180,7 @@
         <v>100000</v>
       </c>
       <c r="Q36" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R36" s="90"/>
       <c r="S36" s="90"/>
@@ -15186,7 +15192,7 @@
         <v>100000</v>
       </c>
       <c r="W36" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X36" s="82"/>
       <c r="Y36" s="82"/>
@@ -15221,7 +15227,7 @@
       <c r="BB36" s="36"/>
       <c r="BC36" s="36"/>
       <c r="BD36" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE36" s="36"/>
       <c r="BF36" s="36"/>
@@ -15263,10 +15269,10 @@
       </c>
       <c r="I37" s="35"/>
       <c r="J37" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K37" s="35" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="L37" s="79"/>
       <c r="M37" s="79"/>
@@ -15278,7 +15284,7 @@
         <v>200000</v>
       </c>
       <c r="Q37" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R37" s="90">
         <v>200000</v>
@@ -15287,7 +15293,7 @@
         <v>200000</v>
       </c>
       <c r="T37" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U37" s="88">
         <v>200000</v>
@@ -15296,7 +15302,7 @@
         <v>200000</v>
       </c>
       <c r="W37" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X37" s="82"/>
       <c r="Y37" s="82"/>
@@ -15331,7 +15337,7 @@
       <c r="BB37" s="36"/>
       <c r="BC37" s="36"/>
       <c r="BD37" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE37" s="36"/>
       <c r="BF37" s="36"/>
@@ -15375,10 +15381,10 @@
         <v>94</v>
       </c>
       <c r="J38" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K38" s="35" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L38" s="79"/>
       <c r="M38" s="79"/>
@@ -15425,7 +15431,7 @@
       <c r="BB38" s="36"/>
       <c r="BC38" s="36"/>
       <c r="BD38" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE38" s="36"/>
       <c r="BF38" s="36"/>
@@ -15467,10 +15473,10 @@
         <v>94</v>
       </c>
       <c r="J39" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K39" s="35" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L39" s="79"/>
       <c r="M39" s="79"/>
@@ -15517,7 +15523,7 @@
       <c r="BB39" s="36"/>
       <c r="BC39" s="36"/>
       <c r="BD39" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE39" s="36"/>
       <c r="BF39" s="36"/>
@@ -15561,10 +15567,10 @@
         <v>94</v>
       </c>
       <c r="J40" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K40" s="35" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L40" s="79"/>
       <c r="M40" s="79"/>
@@ -15611,7 +15617,7 @@
       <c r="BB40" s="36"/>
       <c r="BC40" s="36"/>
       <c r="BD40" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE40" s="36"/>
       <c r="BF40" s="36"/>
@@ -15655,10 +15661,10 @@
         <v>94</v>
       </c>
       <c r="J41" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K41" s="35" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L41" s="79"/>
       <c r="M41" s="79"/>
@@ -15705,7 +15711,7 @@
       <c r="BB41" s="36"/>
       <c r="BC41" s="36"/>
       <c r="BD41" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE41" s="36"/>
       <c r="BF41" s="36"/>
@@ -15749,10 +15755,10 @@
         <v>94</v>
       </c>
       <c r="J42" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K42" s="35" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L42" s="79"/>
       <c r="M42" s="79"/>
@@ -15799,7 +15805,7 @@
       <c r="BB42" s="36"/>
       <c r="BC42" s="36"/>
       <c r="BD42" s="36" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="BE42" s="36"/>
       <c r="BF42" s="36"/>
@@ -15841,10 +15847,10 @@
       </c>
       <c r="I43" s="35"/>
       <c r="J43" s="35" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="K43" s="35" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="L43" s="79">
         <v>0</v>
@@ -15853,7 +15859,7 @@
         <v>5760</v>
       </c>
       <c r="N43" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O43" s="76" t="s">
         <v>117</v>
@@ -15862,7 +15868,7 @@
         <v>540</v>
       </c>
       <c r="Q43" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R43" s="91" t="s">
         <v>117</v>
@@ -15871,7 +15877,7 @@
         <v>540</v>
       </c>
       <c r="T43" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U43" s="89" t="s">
         <v>117</v>
@@ -15880,7 +15886,7 @@
         <v>540</v>
       </c>
       <c r="W43" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X43" s="81" t="s">
         <v>481</v>
@@ -15923,7 +15929,7 @@
       <c r="BB43" s="35"/>
       <c r="BC43" s="35"/>
       <c r="BD43" s="31" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="BE43" s="36"/>
       <c r="BF43" s="35"/>
@@ -15965,10 +15971,10 @@
       </c>
       <c r="I44" s="35"/>
       <c r="J44" s="35" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="K44" s="35" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="L44" s="79">
         <v>0</v>
@@ -15977,7 +15983,7 @@
         <v>5760</v>
       </c>
       <c r="N44" s="79" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O44" s="76" t="s">
         <v>117</v>
@@ -15986,7 +15992,7 @@
         <v>540</v>
       </c>
       <c r="Q44" s="87" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="R44" s="91" t="s">
         <v>117</v>
@@ -15995,7 +16001,7 @@
         <v>540</v>
       </c>
       <c r="T44" s="86" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U44" s="89" t="s">
         <v>117</v>
@@ -16004,7 +16010,7 @@
         <v>540</v>
       </c>
       <c r="W44" s="85" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="X44" s="81" t="s">
         <v>483</v>
@@ -16047,7 +16053,7 @@
       <c r="BB44" s="35"/>
       <c r="BC44" s="35"/>
       <c r="BD44" s="31" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="BE44" s="36"/>
       <c r="BF44" s="35"/>
@@ -16089,10 +16095,10 @@
       </c>
       <c r="I45" s="35"/>
       <c r="J45" s="35" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="K45" s="35" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="L45" s="79"/>
       <c r="M45" s="79"/>
@@ -16147,7 +16153,7 @@
       <c r="BB45" s="35"/>
       <c r="BC45" s="35"/>
       <c r="BD45" s="31" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="BE45" s="36"/>
       <c r="BF45" s="35"/>
@@ -16385,16 +16391,16 @@
         <v>331</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="H4" s="53" t="s">
         <v>115</v>
       </c>
       <c r="I4" s="65" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="K4" s="65" t="s">
         <v>332</v>
@@ -16505,97 +16511,97 @@
         <v>337</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="H5" s="52" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="I5" s="52" t="s">
+        <v>666</v>
+      </c>
+      <c r="J5" s="52" t="s">
+        <v>667</v>
+      </c>
+      <c r="K5" s="52" t="s">
         <v>668</v>
       </c>
-      <c r="J5" s="52" t="s">
+      <c r="L5" s="52" t="s">
         <v>669</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="M5" s="52" t="s">
         <v>670</v>
       </c>
-      <c r="L5" s="52" t="s">
+      <c r="N5" s="52" t="s">
         <v>671</v>
       </c>
-      <c r="M5" s="52" t="s">
+      <c r="O5" s="52" t="s">
         <v>672</v>
       </c>
-      <c r="N5" s="52" t="s">
+      <c r="P5" s="52" t="s">
         <v>673</v>
       </c>
-      <c r="O5" s="52" t="s">
+      <c r="Q5" s="52" t="s">
         <v>674</v>
       </c>
-      <c r="P5" s="52" t="s">
-        <v>675</v>
-      </c>
-      <c r="Q5" s="52" t="s">
+      <c r="R5" s="52" t="s">
         <v>676</v>
       </c>
-      <c r="R5" s="52" t="s">
+      <c r="S5" s="52" t="s">
+        <v>677</v>
+      </c>
+      <c r="T5" s="52" t="s">
         <v>678</v>
       </c>
-      <c r="S5" s="52" t="s">
+      <c r="U5" s="52" t="s">
         <v>679</v>
       </c>
-      <c r="T5" s="52" t="s">
+      <c r="V5" s="52" t="s">
         <v>680</v>
       </c>
-      <c r="U5" s="52" t="s">
+      <c r="W5" s="52" t="s">
         <v>681</v>
       </c>
-      <c r="V5" s="52" t="s">
+      <c r="X5" s="52" t="s">
         <v>682</v>
       </c>
-      <c r="W5" s="52" t="s">
+      <c r="Y5" s="52" t="s">
         <v>683</v>
       </c>
-      <c r="X5" s="52" t="s">
+      <c r="Z5" s="52" t="s">
         <v>684</v>
       </c>
-      <c r="Y5" s="52" t="s">
+      <c r="AA5" s="52" t="s">
         <v>685</v>
       </c>
-      <c r="Z5" s="52" t="s">
+      <c r="AB5" s="52" t="s">
         <v>686</v>
       </c>
-      <c r="AA5" s="52" t="s">
+      <c r="AC5" s="52" t="s">
         <v>687</v>
       </c>
-      <c r="AB5" s="52" t="s">
+      <c r="AD5" s="52" t="s">
         <v>688</v>
       </c>
-      <c r="AC5" s="52" t="s">
+      <c r="AE5" s="52" t="s">
         <v>689</v>
       </c>
-      <c r="AD5" s="52" t="s">
+      <c r="AF5" s="52" t="s">
         <v>690</v>
       </c>
-      <c r="AE5" s="52" t="s">
+      <c r="AG5" s="52" t="s">
         <v>691</v>
       </c>
-      <c r="AF5" s="52" t="s">
+      <c r="AH5" s="52" t="s">
         <v>692</v>
       </c>
-      <c r="AG5" s="52" t="s">
+      <c r="AI5" s="52" t="s">
         <v>693</v>
       </c>
-      <c r="AH5" s="52" t="s">
+      <c r="AJ5" s="52" t="s">
         <v>694</v>
       </c>
-      <c r="AI5" s="52" t="s">
+      <c r="AK5" s="52" t="s">
         <v>695</v>
-      </c>
-      <c r="AJ5" s="52" t="s">
-        <v>696</v>
-      </c>
-      <c r="AK5" s="52" t="s">
-        <v>697</v>
       </c>
       <c r="AL5" s="66" t="s">
         <v>338</v>
@@ -16625,7 +16631,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="54" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="H6" s="54" t="s">
         <v>5</v>
@@ -16744,7 +16750,7 @@
         <v>325</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H7" s="39">
         <v>1</v>
@@ -16855,7 +16861,7 @@
         <v>490</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H8" s="39">
         <v>1</v>
@@ -16966,7 +16972,7 @@
         <v>488</v>
       </c>
       <c r="G9" s="39" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H9" s="39">
         <v>1</v>
@@ -17079,7 +17085,7 @@
         <v>491</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H10" s="39">
         <v>1</v>
@@ -17112,7 +17118,7 @@
         <v>1</v>
       </c>
       <c r="R10" s="69" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="S10" s="69" t="s">
         <v>457</v>
@@ -17192,7 +17198,7 @@
         <v>492</v>
       </c>
       <c r="G11" s="39" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H11" s="39" t="s">
         <v>33</v>
@@ -17309,7 +17315,7 @@
         <v>493</v>
       </c>
       <c r="G12" s="39" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H12" s="39" t="s">
         <v>426</v>
@@ -17428,7 +17434,7 @@
         <v>489</v>
       </c>
       <c r="G13" s="39" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="H13" s="39" t="s">
         <v>426</v>
@@ -17547,7 +17553,7 @@
         <v>494</v>
       </c>
       <c r="G14" s="39" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H14" s="39" t="s">
         <v>426</v>
@@ -17666,7 +17672,7 @@
         <v>495</v>
       </c>
       <c r="G15" s="39" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H15" s="39" t="s">
         <v>426</v>
@@ -17785,7 +17791,7 @@
         <v>496</v>
       </c>
       <c r="G16" s="39" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="H16" s="39" t="s">
         <v>427</v>
@@ -17904,7 +17910,7 @@
         <v>497</v>
       </c>
       <c r="G17" s="39" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H17" s="39" t="s">
         <v>179</v>
@@ -18023,7 +18029,7 @@
         <v>498</v>
       </c>
       <c r="G18" s="39" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H18" s="39" t="s">
         <v>179</v>
@@ -18142,7 +18148,7 @@
         <v>408</v>
       </c>
       <c r="G19" s="39" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="H19" s="39" t="s">
         <v>179</v>
@@ -18261,7 +18267,7 @@
         <v>503</v>
       </c>
       <c r="G20" s="39" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H20" s="39" t="s">
         <v>179</v>
@@ -18380,7 +18386,7 @@
         <v>499</v>
       </c>
       <c r="G21" s="39" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H21" s="39" t="s">
         <v>179</v>
@@ -18499,7 +18505,7 @@
         <v>504</v>
       </c>
       <c r="G22" s="39" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H22" s="39" t="s">
         <v>428</v>
@@ -18618,7 +18624,7 @@
         <v>505</v>
       </c>
       <c r="G23" s="39" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="H23" s="39">
         <v>4</v>
@@ -18737,7 +18743,7 @@
         <v>500</v>
       </c>
       <c r="G24" s="39" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H24" s="39">
         <v>4</v>
@@ -18856,7 +18862,7 @@
         <v>501</v>
       </c>
       <c r="G25" s="39" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H25" s="39">
         <v>4</v>
@@ -18975,7 +18981,7 @@
         <v>502</v>
       </c>
       <c r="G26" s="39" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H26" s="69" t="s">
         <v>93</v>
@@ -19498,7 +19504,7 @@
       <c r="B1" s="164"/>
       <c r="C1" s="164"/>
       <c r="D1" s="131" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E1" s="1"/>
       <c r="H1" s="1"/>
@@ -19511,7 +19517,7 @@
       <c r="B2" s="164"/>
       <c r="C2" s="164"/>
       <c r="D2" s="131" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E2" s="1"/>
       <c r="H2" s="1"/>
@@ -19540,22 +19546,22 @@
         <v>37</v>
       </c>
       <c r="E4" s="128" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F4" s="102" t="s">
         <v>345</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="I4" s="128" t="s">
         <v>247</v>
       </c>
       <c r="J4" s="48" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="K4" s="128" t="s">
         <v>39</v>
@@ -19588,13 +19594,13 @@
         <v>254</v>
       </c>
       <c r="U4" s="116" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="V4" s="116" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="W4" s="116" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="X4" s="80" t="s">
         <v>542</v>
@@ -19612,7 +19618,7 @@
         <v>47</v>
       </c>
       <c r="AC4" s="128" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="AD4" s="128" t="s">
         <v>255</v>
@@ -19639,19 +19645,19 @@
         <v>56</v>
       </c>
       <c r="AL4" s="128" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="AM4" s="128" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="AN4" s="128" t="s">
         <v>57</v>
       </c>
       <c r="AO4" s="128" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="AP4" s="128" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="AQ4" s="128" t="s">
         <v>58</v>
@@ -19684,22 +19690,22 @@
         <v>37</v>
       </c>
       <c r="E5" s="128" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="F5" s="102" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="I5" s="49" t="s">
         <v>259</v>
       </c>
       <c r="J5" s="50" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="K5" s="50" t="s">
         <v>67</v>
@@ -19723,7 +19729,7 @@
         <v>264</v>
       </c>
       <c r="R5" s="49" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="S5" s="132" t="s">
         <v>71</v>
@@ -19732,13 +19738,13 @@
         <v>72</v>
       </c>
       <c r="U5" s="116" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="V5" s="116" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="W5" s="116" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="X5" s="80" t="s">
         <v>541</v>
@@ -19753,16 +19759,16 @@
         <v>73</v>
       </c>
       <c r="AB5" s="49" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="AC5" s="49" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="AD5" s="49" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="AE5" s="49" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="AF5" s="49" t="s">
         <v>265</v>
@@ -19783,19 +19789,19 @@
         <v>82</v>
       </c>
       <c r="AL5" s="49" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="AM5" s="49" t="s">
+        <v>766</v>
+      </c>
+      <c r="AN5" s="49" t="s">
         <v>768</v>
       </c>
-      <c r="AN5" s="49" t="s">
-        <v>770</v>
-      </c>
       <c r="AO5" s="49" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="AP5" s="49" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="AQ5" s="49" t="s">
         <v>83</v>
@@ -19828,7 +19834,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="125" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>5</v>
@@ -19843,7 +19849,7 @@
         <v>5</v>
       </c>
       <c r="J6" s="125" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="K6" s="125" t="s">
         <v>267</v>
@@ -19900,7 +19906,7 @@
         <v>89</v>
       </c>
       <c r="AC6" s="125" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="AD6" s="125" t="s">
         <v>267</v>
@@ -19969,13 +19975,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D7" s="40">
         <v>100</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F7" s="40">
         <v>1</v>
@@ -19984,7 +19990,7 @@
         <v>426</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="I7" s="40">
         <v>20</v>
@@ -20082,13 +20088,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D8" s="40">
         <v>100</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="F8" s="40">
         <v>1</v>
@@ -20097,7 +20103,7 @@
         <v>426</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="I8" s="40">
         <v>20</v>
@@ -20201,7 +20207,7 @@
         <v>102</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F9" s="40">
         <v>6</v>
@@ -20210,7 +20216,7 @@
         <v>426</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="I9" s="40">
         <v>20</v>
@@ -20288,10 +20294,10 @@
       <c r="AL9" s="40"/>
       <c r="AM9" s="40"/>
       <c r="AN9" s="21" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="AO9" s="21" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="AP9" s="21"/>
       <c r="AQ9" s="40" t="s">
@@ -20322,7 +20328,7 @@
         <v>101</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F10" s="40">
         <v>6</v>
@@ -20397,7 +20403,7 @@
       <c r="AN10" s="40"/>
       <c r="AO10" s="40"/>
       <c r="AP10" s="40" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="AQ10" s="40" t="s">
         <v>119</v>
@@ -20427,7 +20433,7 @@
         <v>101</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="F11" s="40">
         <v>6</v>
@@ -20508,11 +20514,11 @@
       <c r="AL11" s="40"/>
       <c r="AM11" s="40"/>
       <c r="AN11" s="43" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="AO11" s="43"/>
       <c r="AP11" s="43" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="AQ11" s="40" t="s">
         <v>94</v>
@@ -20544,7 +20550,7 @@
         <v>101</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F12" s="40">
         <v>6</v>
@@ -20553,7 +20559,7 @@
         <v>426</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="I12" s="40" t="s">
         <v>102</v>
@@ -20635,11 +20641,11 @@
       <c r="AL12" s="40"/>
       <c r="AM12" s="40"/>
       <c r="AN12" s="40" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="AO12" s="40"/>
       <c r="AP12" s="40" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="AQ12" s="40" t="s">
         <v>94</v>
@@ -20671,7 +20677,7 @@
         <v>101</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="F13" s="40">
         <v>6</v>
@@ -20754,11 +20760,11 @@
       <c r="AL13" s="40"/>
       <c r="AM13" s="40"/>
       <c r="AN13" s="43" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="AO13" s="43"/>
       <c r="AP13" s="43" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="AQ13" s="40" t="s">
         <v>119</v>
@@ -20790,7 +20796,7 @@
         <v>101</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="F14" s="40">
         <v>6</v>
@@ -20799,7 +20805,7 @@
         <v>426</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="I14" s="40" t="s">
         <v>125</v>
@@ -20885,11 +20891,11 @@
       </c>
       <c r="AM14" s="40"/>
       <c r="AN14" s="21" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="AO14" s="21"/>
       <c r="AP14" s="21" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="AQ14" s="40" t="s">
         <v>94</v>
@@ -20919,7 +20925,7 @@
         <v>101</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="F15" s="40">
         <v>6</v>
@@ -20928,7 +20934,7 @@
         <v>426</v>
       </c>
       <c r="H15" s="35" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="I15" s="40">
         <v>240</v>
@@ -21014,11 +21020,11 @@
       </c>
       <c r="AM15" s="40"/>
       <c r="AN15" s="21" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="AO15" s="21"/>
       <c r="AP15" s="21" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="AQ15" s="40" t="s">
         <v>94</v>
@@ -21050,7 +21056,7 @@
         <v>101</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F16" s="40">
         <v>6</v>
@@ -21133,11 +21139,11 @@
       </c>
       <c r="AM16" s="40"/>
       <c r="AN16" s="44" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="AO16" s="44"/>
       <c r="AP16" s="44" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="AQ16" s="40" t="s">
         <v>119</v>
@@ -21166,7 +21172,7 @@
         <v>301</v>
       </c>
       <c r="D17" s="45" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E17" s="45"/>
       <c r="F17" s="45">
@@ -21182,7 +21188,7 @@
         <v>302</v>
       </c>
       <c r="J17" s="45" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="K17" s="45" t="s">
         <v>303</v>
@@ -21236,10 +21242,10 @@
       <c r="AL17" s="45"/>
       <c r="AM17" s="45"/>
       <c r="AN17" s="45" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="AO17" s="45" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="AP17" s="45"/>
       <c r="AQ17" s="45" t="s">
@@ -21267,7 +21273,7 @@
         <v>306</v>
       </c>
       <c r="D18" s="45" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E18" s="45"/>
       <c r="F18" s="45">
@@ -21283,7 +21289,7 @@
         <v>302</v>
       </c>
       <c r="J18" s="45" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="K18" s="45" t="s">
         <v>307</v>
@@ -21337,7 +21343,7 @@
       <c r="AL18" s="45"/>
       <c r="AM18" s="45"/>
       <c r="AN18" s="45" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="AO18" s="45"/>
       <c r="AP18" s="45"/>
@@ -21366,7 +21372,7 @@
         <v>310</v>
       </c>
       <c r="D19" s="45" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E19" s="45"/>
       <c r="F19" s="45">
@@ -21376,13 +21382,13 @@
         <v>426</v>
       </c>
       <c r="H19" s="35" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="I19" s="45" t="s">
         <v>302</v>
       </c>
       <c r="J19" s="45" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="K19" s="45" t="s">
         <v>311</v>
@@ -21442,7 +21448,7 @@
       <c r="AL19" s="45"/>
       <c r="AM19" s="45"/>
       <c r="AN19" s="45" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="AO19" s="45"/>
       <c r="AP19" s="45"/>
@@ -21473,7 +21479,7 @@
         <v>314</v>
       </c>
       <c r="D20" s="45" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E20" s="45"/>
       <c r="F20" s="45">
@@ -21483,13 +21489,13 @@
         <v>426</v>
       </c>
       <c r="H20" s="35" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="I20" s="45" t="s">
         <v>302</v>
       </c>
       <c r="J20" s="45" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="K20" s="45" t="s">
         <v>315</v>
@@ -21547,7 +21553,7 @@
       </c>
       <c r="AM20" s="45"/>
       <c r="AN20" s="45" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="AO20" s="45"/>
       <c r="AP20" s="45"/>
@@ -21578,7 +21584,7 @@
         <v>320</v>
       </c>
       <c r="D21" s="45" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E21" s="45"/>
       <c r="F21" s="45">
@@ -21588,13 +21594,13 @@
         <v>426</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="I21" s="45" t="s">
         <v>302</v>
       </c>
       <c r="J21" s="45" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="K21" s="45" t="s">
         <v>321</v>
@@ -21652,7 +21658,7 @@
       </c>
       <c r="AM21" s="45"/>
       <c r="AN21" s="45" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="AO21" s="45"/>
       <c r="AP21" s="45"/>
@@ -21680,10 +21686,10 @@
         <v>16</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="D22" s="45" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E22" s="45"/>
       <c r="F22" s="45">
@@ -21693,13 +21699,13 @@
         <v>426</v>
       </c>
       <c r="H22" s="35" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="I22" s="45" t="s">
         <v>302</v>
       </c>
       <c r="J22" s="45" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="K22" s="45" t="s">
         <v>324</v>
@@ -21759,7 +21765,7 @@
       <c r="AL22" s="45"/>
       <c r="AM22" s="45"/>
       <c r="AN22" s="45" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="AO22" s="45"/>
       <c r="AP22" s="45"/>
@@ -21846,7 +21852,7 @@
       <c r="B1" s="165"/>
       <c r="C1" s="165"/>
       <c r="D1" s="167" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="E1" s="167"/>
       <c r="F1" s="167"/>
@@ -21859,7 +21865,7 @@
       <c r="B2" s="165"/>
       <c r="C2" s="165"/>
       <c r="D2" s="167" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E2" s="167"/>
       <c r="F2" s="167"/>
@@ -21880,61 +21886,61 @@
         <v>2</v>
       </c>
       <c r="C4" s="142" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="D4" s="152" t="s">
+        <v>857</v>
+      </c>
+      <c r="E4" s="153" t="s">
+        <v>858</v>
+      </c>
+      <c r="F4" s="153" t="s">
         <v>859</v>
       </c>
-      <c r="E4" s="153" t="s">
+      <c r="G4" s="153" t="s">
+        <v>895</v>
+      </c>
+      <c r="H4" s="153" t="s">
+        <v>861</v>
+      </c>
+      <c r="I4" s="153" t="s">
+        <v>933</v>
+      </c>
+      <c r="J4" s="153" t="s">
         <v>860</v>
       </c>
-      <c r="F4" s="153" t="s">
-        <v>861</v>
-      </c>
-      <c r="G4" s="153" t="s">
-        <v>897</v>
-      </c>
-      <c r="H4" s="153" t="s">
+      <c r="K4" s="153" t="s">
+        <v>862</v>
+      </c>
+      <c r="L4" s="153" t="s">
         <v>863</v>
       </c>
-      <c r="I4" s="153" t="s">
-        <v>935</v>
-      </c>
-      <c r="J4" s="153" t="s">
-        <v>862</v>
-      </c>
-      <c r="K4" s="153" t="s">
+      <c r="M4" s="153" t="s">
+        <v>924</v>
+      </c>
+      <c r="N4" s="153" t="s">
         <v>864</v>
       </c>
-      <c r="L4" s="153" t="s">
+      <c r="O4" s="153" t="s">
         <v>865</v>
       </c>
-      <c r="M4" s="153" t="s">
-        <v>926</v>
-      </c>
-      <c r="N4" s="153" t="s">
+      <c r="P4" s="153" t="s">
         <v>866</v>
       </c>
-      <c r="O4" s="153" t="s">
+      <c r="Q4" s="153" t="s">
         <v>867</v>
       </c>
-      <c r="P4" s="153" t="s">
+      <c r="R4" s="153" t="s">
         <v>868</v>
       </c>
-      <c r="Q4" s="153" t="s">
+      <c r="S4" s="153" t="s">
         <v>869</v>
       </c>
-      <c r="R4" s="153" t="s">
+      <c r="T4" s="153" t="s">
         <v>870</v>
       </c>
-      <c r="S4" s="153" t="s">
+      <c r="U4" s="153" t="s">
         <v>871</v>
-      </c>
-      <c r="T4" s="153" t="s">
-        <v>872</v>
-      </c>
-      <c r="U4" s="153" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="141" customFormat="1" ht="46" customHeight="1">
@@ -21943,61 +21949,61 @@
         <v>2</v>
       </c>
       <c r="C5" s="144" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D5" s="154" t="s">
+        <v>872</v>
+      </c>
+      <c r="E5" s="154" t="s">
+        <v>873</v>
+      </c>
+      <c r="F5" s="154" t="s">
         <v>874</v>
       </c>
-      <c r="E5" s="154" t="s">
+      <c r="G5" s="154" t="s">
+        <v>782</v>
+      </c>
+      <c r="H5" s="154" t="s">
+        <v>877</v>
+      </c>
+      <c r="I5" s="154" t="s">
         <v>875</v>
       </c>
-      <c r="F5" s="154" t="s">
+      <c r="J5" s="154" t="s">
         <v>876</v>
       </c>
-      <c r="G5" s="154" t="s">
-        <v>784</v>
-      </c>
-      <c r="H5" s="154" t="s">
+      <c r="K5" s="154" t="s">
+        <v>878</v>
+      </c>
+      <c r="L5" s="154" t="s">
         <v>879</v>
       </c>
-      <c r="I5" s="154" t="s">
-        <v>877</v>
-      </c>
-      <c r="J5" s="154" t="s">
-        <v>878</v>
-      </c>
-      <c r="K5" s="154" t="s">
+      <c r="M5" s="154" t="s">
+        <v>928</v>
+      </c>
+      <c r="N5" s="154" t="s">
         <v>880</v>
       </c>
-      <c r="L5" s="154" t="s">
+      <c r="O5" s="154" t="s">
         <v>881</v>
       </c>
-      <c r="M5" s="154" t="s">
-        <v>930</v>
-      </c>
-      <c r="N5" s="154" t="s">
+      <c r="P5" s="154" t="s">
         <v>882</v>
       </c>
-      <c r="O5" s="154" t="s">
+      <c r="Q5" s="154" t="s">
         <v>883</v>
       </c>
-      <c r="P5" s="154" t="s">
+      <c r="R5" s="154" t="s">
         <v>884</v>
       </c>
-      <c r="Q5" s="154" t="s">
+      <c r="S5" s="154" t="s">
+        <v>896</v>
+      </c>
+      <c r="T5" s="154" t="s">
         <v>885</v>
       </c>
-      <c r="R5" s="154" t="s">
+      <c r="U5" s="154" t="s">
         <v>886</v>
-      </c>
-      <c r="S5" s="154" t="s">
-        <v>898</v>
-      </c>
-      <c r="T5" s="154" t="s">
-        <v>887</v>
-      </c>
-      <c r="U5" s="154" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="141" customFormat="1" ht="21" customHeight="1">
@@ -22036,7 +22042,7 @@
         <v>89</v>
       </c>
       <c r="M6" s="155" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="N6" s="155" t="s">
         <v>89</v>
@@ -22065,23 +22071,23 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="148" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B7" s="137">
         <v>1</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D7" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E7" s="137" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="F7" s="151"/>
       <c r="G7" s="137" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="H7" s="151"/>
       <c r="I7" s="151"/>
@@ -22096,34 +22102,34 @@
       <c r="P7" s="151"/>
       <c r="Q7" s="151"/>
       <c r="R7" s="137" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="S7" s="138"/>
       <c r="T7" s="151"/>
       <c r="U7" s="151"/>
       <c r="V7" s="136" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="148" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B8" s="137">
         <v>2</v>
       </c>
       <c r="C8" s="137" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D8" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E8" s="137" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="F8" s="151"/>
       <c r="G8" s="137" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="H8" s="151"/>
       <c r="I8" s="151"/>
@@ -22138,20 +22144,20 @@
       <c r="P8" s="151"/>
       <c r="Q8" s="151"/>
       <c r="R8" s="137" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="S8" s="138"/>
       <c r="T8" s="156" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="U8" s="151"/>
       <c r="V8" s="136" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="148" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B9" s="137">
         <v>3</v>
@@ -22160,14 +22166,14 @@
         <v>194</v>
       </c>
       <c r="D9" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E9" s="137" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="F9" s="151"/>
       <c r="G9" s="137" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="H9" s="151"/>
       <c r="I9" s="151">
@@ -22176,7 +22182,7 @@
       <c r="J9" s="151"/>
       <c r="K9" s="151"/>
       <c r="L9" s="39" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="M9" s="39"/>
       <c r="N9" s="151"/>
@@ -22186,34 +22192,34 @@
       <c r="P9" s="151"/>
       <c r="Q9" s="151"/>
       <c r="R9" s="137" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="S9" s="138"/>
       <c r="T9" s="151"/>
       <c r="U9" s="151"/>
       <c r="V9" s="136" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="148" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="B10" s="137">
         <v>4</v>
       </c>
       <c r="C10" s="137" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D10" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E10" s="137" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="F10" s="151"/>
       <c r="G10" s="137" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="H10" s="151"/>
       <c r="I10" s="151">
@@ -22222,10 +22228,10 @@
       <c r="J10" s="151"/>
       <c r="K10" s="151"/>
       <c r="L10" s="39" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="M10" s="39" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="N10" s="151"/>
       <c r="O10" s="163" t="s">
@@ -22234,71 +22240,71 @@
       <c r="P10" s="151"/>
       <c r="Q10" s="151"/>
       <c r="R10" s="137" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="S10" s="138"/>
       <c r="T10" s="151"/>
       <c r="U10" s="151"/>
       <c r="V10" s="136" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="148" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B11" s="137">
         <v>5</v>
       </c>
       <c r="C11" s="137" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D11" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E11" s="137" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="F11" s="151"/>
       <c r="G11" s="137" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="H11" s="151"/>
       <c r="I11" s="151"/>
       <c r="J11" s="151"/>
       <c r="K11" s="151"/>
       <c r="L11" s="39" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="M11" s="39"/>
       <c r="N11" s="151"/>
       <c r="O11" s="39" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="P11" s="151"/>
       <c r="Q11" s="151"/>
       <c r="R11" s="137" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="S11" s="138"/>
       <c r="T11" s="151"/>
       <c r="U11" s="151"/>
       <c r="V11" s="136" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="148" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="B12" s="137">
         <v>6</v>
       </c>
       <c r="C12" s="137" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D12" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E12" s="137"/>
       <c r="F12" s="151"/>
@@ -22308,7 +22314,7 @@
       <c r="J12" s="151"/>
       <c r="K12" s="151"/>
       <c r="L12" s="39" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="M12" s="39"/>
       <c r="N12" s="151"/>
@@ -22320,109 +22326,109 @@
       <c r="T12" s="151"/>
       <c r="U12" s="151"/>
       <c r="V12" s="136" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="148" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="B13" s="137">
         <v>7</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D13" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E13" s="137" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="F13" s="151"/>
       <c r="G13" s="39" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="H13" s="151"/>
       <c r="I13" s="151"/>
       <c r="J13" s="151"/>
       <c r="K13" s="151"/>
       <c r="L13" s="39" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="M13" s="39"/>
       <c r="N13" s="151"/>
       <c r="O13" s="39" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="P13" s="151"/>
       <c r="Q13" s="151"/>
       <c r="R13" s="137" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="S13" s="138"/>
       <c r="T13" s="151"/>
       <c r="U13" s="151"/>
       <c r="V13" s="136" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="148" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B14" s="137">
         <v>8</v>
       </c>
       <c r="C14" s="137" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D14" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E14" s="137" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="F14" s="151"/>
       <c r="G14" s="137" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="H14" s="151"/>
       <c r="I14" s="151"/>
       <c r="J14" s="151"/>
       <c r="K14" s="151"/>
       <c r="L14" s="39" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="M14" s="39"/>
       <c r="N14" s="151"/>
       <c r="O14" s="39" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="P14" s="151"/>
       <c r="Q14" s="151"/>
       <c r="R14" s="137" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="S14" s="138"/>
       <c r="T14" s="151"/>
       <c r="U14" s="151"/>
       <c r="V14" s="139" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="148" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B15" s="39" t="s">
         <v>113</v>
       </c>
       <c r="C15" s="137" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="D15" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E15" s="137"/>
       <c r="F15" s="151"/>
@@ -22451,17 +22457,17 @@
         <v>97</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D16" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E16" s="137" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="F16" s="151"/>
       <c r="G16" s="137" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="H16" s="151"/>
       <c r="I16" s="151"/>
@@ -22479,22 +22485,22 @@
       <c r="S16" s="138"/>
       <c r="T16" s="151"/>
       <c r="U16" s="156" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="V16" s="140"/>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="149" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B17" s="137" t="s">
         <v>135</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D17" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E17" s="137" t="s">
         <v>150</v>
@@ -22516,7 +22522,7 @@
       <c r="P17" s="151"/>
       <c r="Q17" s="151"/>
       <c r="R17" s="137" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="S17" s="138"/>
       <c r="T17" s="151"/>
@@ -22525,16 +22531,16 @@
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="149" t="s">
+        <v>811</v>
+      </c>
+      <c r="B18" s="137" t="s">
         <v>813</v>
       </c>
-      <c r="B18" s="137" t="s">
-        <v>815</v>
-      </c>
       <c r="C18" s="137" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D18" s="137" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E18" s="137" t="s">
         <v>150</v>
@@ -22556,7 +22562,7 @@
       <c r="P18" s="151"/>
       <c r="Q18" s="151"/>
       <c r="R18" s="137" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="S18" s="138"/>
       <c r="T18" s="151"/>

</xml_diff>